<commit_message>
Adding a new error class + reviewing annotation
</commit_message>
<xml_diff>
--- a/data/results/all_lemmas_annotated.xlsx
+++ b/data/results/all_lemmas_annotated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/27f43607ae8ba673/Dokumenty/GitHub/ma-thesis-swe/data/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_12592DBC445CD00F62355476585DCE3A8746B9DD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAF17C05-69D3-42CA-98B2-9E66059A3E03}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="11_12592DBC445CD00F62355476585DCE3A8746B9DD" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{853FCB07-4C74-4686-A5A1-E92F99CC3CDD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="523">
   <si>
     <t>Token</t>
   </si>
@@ -1586,6 +1586,9 @@
   </si>
   <si>
     <t>foreign</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -1657,7 +1660,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1675,6 +1678,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1965,7 +1972,7 @@
   <dimension ref="A1:G146"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2386,7 +2393,7 @@
         <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -3168,7 +3175,7 @@
         <v>199</v>
       </c>
       <c r="G52" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3191,7 +3198,7 @@
         <v>69</v>
       </c>
       <c r="G53" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3260,7 +3267,7 @@
         <v>210</v>
       </c>
       <c r="G56" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3651,7 +3658,7 @@
         <v>278</v>
       </c>
       <c r="G73" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3881,7 +3888,7 @@
         <v>306</v>
       </c>
       <c r="G83" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4065,7 +4072,7 @@
         <v>332</v>
       </c>
       <c r="G91" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>